<commit_message>
Huge bugfix that fixed the problem where we could not read the same file multiple times
</commit_message>
<xml_diff>
--- a/docs/milestones.xlsx
+++ b/docs/milestones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14740"/>
+    <workbookView minimized="1" xWindow="6400" yWindow="6060" windowWidth="25600" windowHeight="14740"/>
   </bookViews>
   <sheets>
     <sheet name="task list" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>Line Item</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Initial Project Setup and build tools</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -644,7 +650,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -704,7 +710,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -722,7 +728,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F4" s="5"/>
     </row>
@@ -740,7 +746,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F5" s="5"/>
     </row>
@@ -758,7 +764,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F6" s="5"/>
     </row>

</xml_diff>